<commit_message>
Last week before rest week
</commit_message>
<xml_diff>
--- a/frames.xlsx
+++ b/frames.xlsx
@@ -339,7 +339,7 @@
   <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G49" activeCellId="0" sqref="G49"/>
+      <selection pane="topLeft" activeCell="G51" activeCellId="0" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1350,6 +1350,9 @@
       <c r="F50" s="0" t="n">
         <v>11</v>
       </c>
+      <c r="G50" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">

</xml_diff>